<commit_message>
Added team abbreviations and teams not playing this year (2020/2021)
</commit_message>
<xml_diff>
--- a/Logos.xlsx
+++ b/Logos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3712,8 +3712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C359"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A335" workbookViewId="0">
-      <selection activeCell="C363" sqref="C363"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Changed NCAA logo to the dedicated NCAA basketball logo
</commit_message>
<xml_diff>
--- a/Logos.xlsx
+++ b/Logos.xlsx
@@ -2082,9 +2082,6 @@
     <t>https://a4.espncdn.com/combiner/i?img=%2Fi%2Fteamlogos%2Fncaa%2F500%2F2132.png</t>
   </si>
   <si>
-    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/d/dd/NCAA_logo.svg/1042px-NCAA_logo.svg.png</t>
-  </si>
-  <si>
     <t>NCAA</t>
   </si>
   <si>
@@ -3724,6 +3721,9 @@
   </si>
   <si>
     <t>https://upload.wikimedia.org/wikipedia/en/thumb/4/40/Boise_State_Broncos_logo.svg/1200px-Boise_State_Broncos_logo.svg.png</t>
+  </si>
+  <si>
+    <t>https://cdn.freebiesupply.com/logos/large/2x/ncaa-basketball-logo-png-transparent.png</t>
   </si>
 </sst>
 </file>
@@ -5215,8 +5215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D359"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5231,10 +5231,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -5242,16 +5242,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D2" t="s">
-        <v>687</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5259,10 +5259,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C3" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -5276,7 +5276,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -5290,7 +5290,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -5304,7 +5304,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D6" t="s">
         <v>352</v>
@@ -5315,10 +5315,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C7" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D7" t="s">
         <v>353</v>
@@ -5329,10 +5329,10 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C8" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D8" t="s">
         <v>354</v>
@@ -5346,7 +5346,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D9" t="s">
         <v>355</v>
@@ -5357,10 +5357,10 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="C10" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D10" t="s">
         <v>356</v>
@@ -5374,7 +5374,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D11" t="s">
         <v>357</v>
@@ -5385,10 +5385,10 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C12" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D12" t="s">
         <v>358</v>
@@ -5402,7 +5402,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D13" t="s">
         <v>359</v>
@@ -5413,10 +5413,10 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="C14" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D14" t="s">
         <v>360</v>
@@ -5430,7 +5430,7 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D15" t="s">
         <v>361</v>
@@ -5441,10 +5441,10 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="C16" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D16" t="s">
         <v>362</v>
@@ -5455,13 +5455,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="C17" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D17" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -5472,7 +5472,7 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D18" t="s">
         <v>363</v>
@@ -5486,7 +5486,7 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D19" t="s">
         <v>364</v>
@@ -5500,7 +5500,7 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D20" t="s">
         <v>365</v>
@@ -5511,10 +5511,10 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="C21" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D21" t="s">
         <v>366</v>
@@ -5528,7 +5528,7 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D22" t="s">
         <v>367</v>
@@ -5542,7 +5542,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D23" t="s">
         <v>368</v>
@@ -5556,7 +5556,7 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D24" t="s">
         <v>369</v>
@@ -5564,16 +5564,16 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C25" t="s">
         <v>719</v>
       </c>
-      <c r="B25" t="s">
-        <v>1068</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>720</v>
-      </c>
-      <c r="D25" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5584,7 +5584,7 @@
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D26" t="s">
         <v>370</v>
@@ -5595,13 +5595,13 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="C27" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D27" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5609,10 +5609,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="C28" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D28" t="s">
         <v>371</v>
@@ -5623,10 +5623,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="C29" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D29" t="s">
         <v>372</v>
@@ -5637,10 +5637,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="C30" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D30" t="s">
         <v>373</v>
@@ -5648,16 +5648,16 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="B31" t="s">
+        <v>727</v>
+      </c>
+      <c r="C31" t="s">
         <v>728</v>
       </c>
-      <c r="B31" t="s">
-        <v>728</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>729</v>
-      </c>
-      <c r="D31" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5668,7 +5668,7 @@
         <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D32" t="s">
         <v>374</v>
@@ -5682,7 +5682,7 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D33" t="s">
         <v>375</v>
@@ -5696,7 +5696,7 @@
         <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D34" t="s">
         <v>376</v>
@@ -5710,7 +5710,7 @@
         <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D35" t="s">
         <v>377</v>
@@ -5724,7 +5724,7 @@
         <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D36" t="s">
         <v>378</v>
@@ -5752,7 +5752,7 @@
         <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D38" t="s">
         <v>380</v>
@@ -5766,7 +5766,7 @@
         <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D39" t="s">
         <v>381</v>
@@ -5777,10 +5777,10 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D40" t="s">
         <v>382</v>
@@ -5791,10 +5791,10 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="C41" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D41" t="s">
         <v>383</v>
@@ -5805,10 +5805,10 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C42" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D42" t="s">
         <v>384</v>
@@ -5822,7 +5822,7 @@
         <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D43" t="s">
         <v>385</v>
@@ -5836,7 +5836,7 @@
         <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="D44" t="s">
         <v>386</v>
@@ -5850,7 +5850,7 @@
         <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D45" t="s">
         <v>387</v>
@@ -5861,10 +5861,10 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="C46" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D46" t="s">
         <v>388</v>
@@ -5875,10 +5875,10 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="C47" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D47" t="s">
         <v>389</v>
@@ -5889,10 +5889,10 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C48" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D48" t="s">
         <v>390</v>
@@ -5903,10 +5903,10 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C49" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D49" t="s">
         <v>391</v>
@@ -5920,7 +5920,7 @@
         <v>50</v>
       </c>
       <c r="C50" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D50" t="s">
         <v>392</v>
@@ -5934,7 +5934,7 @@
         <v>51</v>
       </c>
       <c r="C51" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D51" t="s">
         <v>393</v>
@@ -5945,13 +5945,13 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C52" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D52" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -5962,7 +5962,7 @@
         <v>53</v>
       </c>
       <c r="C53" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D53" t="s">
         <v>686</v>
@@ -5976,7 +5976,7 @@
         <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="D54" t="s">
         <v>394</v>
@@ -5987,10 +5987,10 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="C55" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D55" t="s">
         <v>395</v>
@@ -6001,10 +6001,10 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="C56" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D56" t="s">
         <v>396</v>
@@ -6018,7 +6018,7 @@
         <v>57</v>
       </c>
       <c r="C57" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D57" t="s">
         <v>397</v>
@@ -6029,10 +6029,10 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C58" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D58" t="s">
         <v>398</v>
@@ -6046,7 +6046,7 @@
         <v>59</v>
       </c>
       <c r="C59" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D59" t="s">
         <v>399</v>
@@ -6057,10 +6057,10 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="C60" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D60" t="s">
         <v>400</v>
@@ -6068,16 +6068,16 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="B61" t="s">
+        <v>758</v>
+      </c>
+      <c r="C61" t="s">
         <v>759</v>
       </c>
-      <c r="B61" t="s">
-        <v>759</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>760</v>
-      </c>
-      <c r="D61" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -6088,7 +6088,7 @@
         <v>61</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="D62" t="s">
         <v>401</v>
@@ -6099,10 +6099,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="C63" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D63" t="s">
         <v>402</v>
@@ -6110,16 +6110,16 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B64" t="s">
+        <v>762</v>
+      </c>
+      <c r="C64" t="s">
         <v>763</v>
       </c>
-      <c r="B64" t="s">
-        <v>763</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>764</v>
-      </c>
-      <c r="D64" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -6130,7 +6130,7 @@
         <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D65" t="s">
         <v>403</v>
@@ -6138,16 +6138,16 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B66" t="s">
+        <v>766</v>
+      </c>
+      <c r="C66" t="s">
         <v>767</v>
       </c>
-      <c r="B66" t="s">
-        <v>767</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>768</v>
-      </c>
-      <c r="D66" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -6158,7 +6158,7 @@
         <v>64</v>
       </c>
       <c r="C67" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D67" t="s">
         <v>405</v>
@@ -6172,7 +6172,7 @@
         <v>65</v>
       </c>
       <c r="C68" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D68" t="s">
         <v>404</v>
@@ -6186,7 +6186,7 @@
         <v>66</v>
       </c>
       <c r="C69" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D69" t="s">
         <v>407</v>
@@ -6197,10 +6197,10 @@
         <v>67</v>
       </c>
       <c r="B70" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="C70" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D70" t="s">
         <v>408</v>
@@ -6214,7 +6214,7 @@
         <v>68</v>
       </c>
       <c r="C71" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D71" t="s">
         <v>409</v>
@@ -6228,7 +6228,7 @@
         <v>69</v>
       </c>
       <c r="C72" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D72" t="s">
         <v>410</v>
@@ -6242,7 +6242,7 @@
         <v>70</v>
       </c>
       <c r="C73" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D73" t="s">
         <v>411</v>
@@ -6253,10 +6253,10 @@
         <v>71</v>
       </c>
       <c r="B74" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="C74" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D74" t="s">
         <v>412</v>
@@ -6270,7 +6270,7 @@
         <v>72</v>
       </c>
       <c r="C75" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D75" t="s">
         <v>413</v>
@@ -6284,7 +6284,7 @@
         <v>73</v>
       </c>
       <c r="C76" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D76" t="s">
         <v>414</v>
@@ -6298,7 +6298,7 @@
         <v>74</v>
       </c>
       <c r="C77" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D77" t="s">
         <v>415</v>
@@ -6312,7 +6312,7 @@
         <v>75</v>
       </c>
       <c r="C78" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D78" t="s">
         <v>416</v>
@@ -6323,10 +6323,10 @@
         <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="C79" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D79" t="s">
         <v>417</v>
@@ -6337,10 +6337,10 @@
         <v>77</v>
       </c>
       <c r="B80" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C80" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D80" t="s">
         <v>418</v>
@@ -6351,10 +6351,10 @@
         <v>78</v>
       </c>
       <c r="B81" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C81" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D81" t="s">
         <v>419</v>
@@ -6365,10 +6365,10 @@
         <v>79</v>
       </c>
       <c r="B82" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C82" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D82" t="s">
         <v>420</v>
@@ -6379,10 +6379,10 @@
         <v>80</v>
       </c>
       <c r="B83" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="C83" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D83" t="s">
         <v>421</v>
@@ -6393,10 +6393,10 @@
         <v>81</v>
       </c>
       <c r="B84" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="C84" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D84" t="s">
         <v>422</v>
@@ -6410,7 +6410,7 @@
         <v>82</v>
       </c>
       <c r="C85" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D85" t="s">
         <v>423</v>
@@ -6424,7 +6424,7 @@
         <v>83</v>
       </c>
       <c r="C86" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="D86" t="s">
         <v>424</v>
@@ -6438,7 +6438,7 @@
         <v>84</v>
       </c>
       <c r="C87" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D87" t="s">
         <v>425</v>
@@ -6449,10 +6449,10 @@
         <v>85</v>
       </c>
       <c r="B88" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="C88" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D88" t="s">
         <v>426</v>
@@ -6463,7 +6463,7 @@
         <v>86</v>
       </c>
       <c r="B89" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="C89" t="s">
         <v>86</v>
@@ -6480,7 +6480,7 @@
         <v>87</v>
       </c>
       <c r="C90" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="D90" t="s">
         <v>428</v>
@@ -6494,7 +6494,7 @@
         <v>88</v>
       </c>
       <c r="C91" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D91" t="s">
         <v>429</v>
@@ -6505,10 +6505,10 @@
         <v>89</v>
       </c>
       <c r="B92" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C92" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D92" t="s">
         <v>430</v>
@@ -6519,10 +6519,10 @@
         <v>90</v>
       </c>
       <c r="B93" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="C93" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D93" t="s">
         <v>431</v>
@@ -6533,10 +6533,10 @@
         <v>91</v>
       </c>
       <c r="B94" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="C94" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D94" t="s">
         <v>432</v>
@@ -6550,7 +6550,7 @@
         <v>92</v>
       </c>
       <c r="C95" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D95" t="s">
         <v>433</v>
@@ -6561,10 +6561,10 @@
         <v>93</v>
       </c>
       <c r="B96" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D96" t="s">
         <v>406</v>
@@ -6575,10 +6575,10 @@
         <v>94</v>
       </c>
       <c r="B97" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C97" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D97" t="s">
         <v>434</v>
@@ -6592,10 +6592,10 @@
         <v>95</v>
       </c>
       <c r="C98" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D98" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -6603,10 +6603,10 @@
         <v>96</v>
       </c>
       <c r="B99" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C99" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D99" t="s">
         <v>435</v>
@@ -6617,10 +6617,10 @@
         <v>97</v>
       </c>
       <c r="B100" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C100" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D100" t="s">
         <v>436</v>
@@ -6631,10 +6631,10 @@
         <v>98</v>
       </c>
       <c r="B101" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C101" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D101" t="s">
         <v>437</v>
@@ -6648,7 +6648,7 @@
         <v>99</v>
       </c>
       <c r="C102" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D102" t="s">
         <v>438</v>
@@ -6662,7 +6662,7 @@
         <v>100</v>
       </c>
       <c r="C103" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D103" t="s">
         <v>439</v>
@@ -6673,10 +6673,10 @@
         <v>101</v>
       </c>
       <c r="B104" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="C104" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D104" t="s">
         <v>440</v>
@@ -6687,10 +6687,10 @@
         <v>102</v>
       </c>
       <c r="B105" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="C105" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D105" t="s">
         <v>441</v>
@@ -6701,10 +6701,10 @@
         <v>103</v>
       </c>
       <c r="B106" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="C106" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D106" t="s">
         <v>442</v>
@@ -6718,7 +6718,7 @@
         <v>104</v>
       </c>
       <c r="C107" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D107" t="s">
         <v>408</v>
@@ -6729,10 +6729,10 @@
         <v>105</v>
       </c>
       <c r="B108" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="C108" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D108" t="s">
         <v>443</v>
@@ -6743,10 +6743,10 @@
         <v>106</v>
       </c>
       <c r="B109" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C109" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D109" t="s">
         <v>444</v>
@@ -6757,13 +6757,13 @@
         <v>107</v>
       </c>
       <c r="B110" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="C110" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D110" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -6774,7 +6774,7 @@
         <v>108</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D111" t="s">
         <v>445</v>
@@ -6788,7 +6788,7 @@
         <v>109</v>
       </c>
       <c r="C112" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="D112" t="s">
         <v>446</v>
@@ -6796,16 +6796,16 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B113" t="s">
+        <v>813</v>
+      </c>
+      <c r="C113" t="s">
+        <v>815</v>
+      </c>
+      <c r="D113" t="s">
         <v>814</v>
-      </c>
-      <c r="B113" t="s">
-        <v>814</v>
-      </c>
-      <c r="C113" t="s">
-        <v>816</v>
-      </c>
-      <c r="D113" t="s">
-        <v>815</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -6816,7 +6816,7 @@
         <v>110</v>
       </c>
       <c r="C114" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="D114" t="s">
         <v>447</v>
@@ -6830,7 +6830,7 @@
         <v>111</v>
       </c>
       <c r="C115" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D115" t="s">
         <v>448</v>
@@ -6844,7 +6844,7 @@
         <v>112</v>
       </c>
       <c r="C116" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D116" t="s">
         <v>449</v>
@@ -6858,7 +6858,7 @@
         <v>113</v>
       </c>
       <c r="C117" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="D117" t="s">
         <v>450</v>
@@ -6872,7 +6872,7 @@
         <v>114</v>
       </c>
       <c r="C118" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D118" t="s">
         <v>451</v>
@@ -6883,10 +6883,10 @@
         <v>115</v>
       </c>
       <c r="B119" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="C119" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="D119" t="s">
         <v>452</v>
@@ -6900,7 +6900,7 @@
         <v>116</v>
       </c>
       <c r="C120" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="D120" t="s">
         <v>453</v>
@@ -6914,7 +6914,7 @@
         <v>117</v>
       </c>
       <c r="C121" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D121" t="s">
         <v>454</v>
@@ -6925,10 +6925,10 @@
         <v>118</v>
       </c>
       <c r="B122" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="C122" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D122" t="s">
         <v>455</v>
@@ -6942,7 +6942,7 @@
         <v>119</v>
       </c>
       <c r="C123" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D123" t="s">
         <v>456</v>
@@ -6953,10 +6953,10 @@
         <v>120</v>
       </c>
       <c r="B124" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="C124" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D124" t="s">
         <v>457</v>
@@ -6967,10 +6967,10 @@
         <v>121</v>
       </c>
       <c r="B125" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="C125" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D125" t="s">
         <v>458</v>
@@ -6981,10 +6981,10 @@
         <v>122</v>
       </c>
       <c r="B126" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C126" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="D126" t="s">
         <v>459</v>
@@ -6998,7 +6998,7 @@
         <v>123</v>
       </c>
       <c r="C127" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D127" t="s">
         <v>460</v>
@@ -7009,10 +7009,10 @@
         <v>124</v>
       </c>
       <c r="B128" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C128" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D128" t="s">
         <v>461</v>
@@ -7026,7 +7026,7 @@
         <v>125</v>
       </c>
       <c r="C129" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="D129" t="s">
         <v>462</v>
@@ -7040,7 +7040,7 @@
         <v>126</v>
       </c>
       <c r="C130" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D130" t="s">
         <v>463</v>
@@ -7051,10 +7051,10 @@
         <v>127</v>
       </c>
       <c r="B131" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="C131" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D131" t="s">
         <v>464</v>
@@ -7068,7 +7068,7 @@
         <v>128</v>
       </c>
       <c r="C132" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D132" t="s">
         <v>465</v>
@@ -7079,10 +7079,10 @@
         <v>129</v>
       </c>
       <c r="B133" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="C133" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="D133" t="s">
         <v>466</v>
@@ -7096,7 +7096,7 @@
         <v>130</v>
       </c>
       <c r="C134" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="D134" t="s">
         <v>467</v>
@@ -7107,10 +7107,10 @@
         <v>131</v>
       </c>
       <c r="B135" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C135" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D135" t="s">
         <v>468</v>
@@ -7121,10 +7121,10 @@
         <v>132</v>
       </c>
       <c r="B136" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C136" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D136" t="s">
         <v>469</v>
@@ -7138,7 +7138,7 @@
         <v>133</v>
       </c>
       <c r="C137" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D137" t="s">
         <v>470</v>
@@ -7149,10 +7149,10 @@
         <v>134</v>
       </c>
       <c r="B138" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C138" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D138" t="s">
         <v>471</v>
@@ -7163,10 +7163,10 @@
         <v>135</v>
       </c>
       <c r="B139" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C139" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="D139" t="s">
         <v>472</v>
@@ -7177,10 +7177,10 @@
         <v>136</v>
       </c>
       <c r="B140" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C140" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="D140" t="s">
         <v>473</v>
@@ -7194,7 +7194,7 @@
         <v>137</v>
       </c>
       <c r="C141" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="D141" t="s">
         <v>474</v>
@@ -7208,7 +7208,7 @@
         <v>138</v>
       </c>
       <c r="C142" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D142" t="s">
         <v>475</v>
@@ -7222,7 +7222,7 @@
         <v>139</v>
       </c>
       <c r="C143" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D143" t="s">
         <v>476</v>
@@ -7236,7 +7236,7 @@
         <v>140</v>
       </c>
       <c r="C144" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="D144" t="s">
         <v>477</v>
@@ -7250,7 +7250,7 @@
         <v>141</v>
       </c>
       <c r="C145" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D145" t="s">
         <v>478</v>
@@ -7264,7 +7264,7 @@
         <v>142</v>
       </c>
       <c r="C146" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D146" t="s">
         <v>479</v>
@@ -7278,7 +7278,7 @@
         <v>143</v>
       </c>
       <c r="C147" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D147" t="s">
         <v>682</v>
@@ -7289,10 +7289,10 @@
         <v>144</v>
       </c>
       <c r="B148" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C148" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D148" t="s">
         <v>683</v>
@@ -7303,10 +7303,10 @@
         <v>145</v>
       </c>
       <c r="B149" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C149" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D149" t="s">
         <v>684</v>
@@ -7317,10 +7317,10 @@
         <v>146</v>
       </c>
       <c r="B150" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C150" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="D150" t="s">
         <v>685</v>
@@ -7334,7 +7334,7 @@
         <v>147</v>
       </c>
       <c r="C151" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="D151" t="s">
         <v>480</v>
@@ -7345,10 +7345,10 @@
         <v>148</v>
       </c>
       <c r="B152" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C152" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D152" t="s">
         <v>481</v>
@@ -7359,10 +7359,10 @@
         <v>149</v>
       </c>
       <c r="B153" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C153" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="D153" t="s">
         <v>482</v>
@@ -7373,10 +7373,10 @@
         <v>150</v>
       </c>
       <c r="B154" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="C154" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="D154" t="s">
         <v>483</v>
@@ -7390,7 +7390,7 @@
         <v>151</v>
       </c>
       <c r="C155" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="D155" t="s">
         <v>484</v>
@@ -7401,10 +7401,10 @@
         <v>152</v>
       </c>
       <c r="B156" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="C156" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D156" t="s">
         <v>485</v>
@@ -7415,10 +7415,10 @@
         <v>153</v>
       </c>
       <c r="B157" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="C157" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="D157" t="s">
         <v>486</v>
@@ -7429,10 +7429,10 @@
         <v>154</v>
       </c>
       <c r="B158" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="C158" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D158" t="s">
         <v>487</v>
@@ -7460,7 +7460,7 @@
         <v>156</v>
       </c>
       <c r="C160" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D160" t="s">
         <v>489</v>
@@ -7474,7 +7474,7 @@
         <v>157</v>
       </c>
       <c r="C161" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D161" t="s">
         <v>490</v>
@@ -7488,7 +7488,7 @@
         <v>158</v>
       </c>
       <c r="C162" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D162" t="s">
         <v>491</v>
@@ -7502,7 +7502,7 @@
         <v>159</v>
       </c>
       <c r="C163" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D163" t="s">
         <v>492</v>
@@ -7516,7 +7516,7 @@
         <v>160</v>
       </c>
       <c r="C164" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D164" t="s">
         <v>493</v>
@@ -7530,7 +7530,7 @@
         <v>161</v>
       </c>
       <c r="C165" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D165" t="s">
         <v>494</v>
@@ -7538,16 +7538,16 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B166" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C166" s="2" t="s">
         <v>1053</v>
       </c>
-      <c r="B166" t="s">
-        <v>1132</v>
-      </c>
-      <c r="C166" s="2" t="s">
+      <c r="D166" t="s">
         <v>1054</v>
-      </c>
-      <c r="D166" t="s">
-        <v>1055</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -7555,10 +7555,10 @@
         <v>162</v>
       </c>
       <c r="B167" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="C167" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="D167" t="s">
         <v>495</v>
@@ -7569,10 +7569,10 @@
         <v>163</v>
       </c>
       <c r="B168" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="C168" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D168" t="s">
         <v>496</v>
@@ -7586,7 +7586,7 @@
         <v>164</v>
       </c>
       <c r="C169" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D169" t="s">
         <v>497</v>
@@ -7600,7 +7600,7 @@
         <v>165</v>
       </c>
       <c r="C170" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="D170" t="s">
         <v>498</v>
@@ -7614,7 +7614,7 @@
         <v>166</v>
       </c>
       <c r="C171" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D171" t="s">
         <v>499</v>
@@ -7625,10 +7625,10 @@
         <v>167</v>
       </c>
       <c r="B172" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="C172" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="D172" t="s">
         <v>500</v>
@@ -7639,10 +7639,10 @@
         <v>168</v>
       </c>
       <c r="B173" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="C173" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="D173" t="s">
         <v>501</v>
@@ -7656,7 +7656,7 @@
         <v>169</v>
       </c>
       <c r="C174" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="D174" t="s">
         <v>502</v>
@@ -7667,10 +7667,10 @@
         <v>170</v>
       </c>
       <c r="B175" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="C175" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="D175" t="s">
         <v>503</v>
@@ -7681,10 +7681,10 @@
         <v>171</v>
       </c>
       <c r="B176" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="C176" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="D176" t="s">
         <v>504</v>
@@ -7695,10 +7695,10 @@
         <v>172</v>
       </c>
       <c r="B177" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="C177" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D177" t="s">
         <v>505</v>
@@ -7712,7 +7712,7 @@
         <v>173</v>
       </c>
       <c r="C178" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D178" t="s">
         <v>506</v>
@@ -7726,7 +7726,7 @@
         <v>174</v>
       </c>
       <c r="C179" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D179" t="s">
         <v>507</v>
@@ -7737,10 +7737,10 @@
         <v>175</v>
       </c>
       <c r="B180" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="C180" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D180" t="s">
         <v>508</v>
@@ -7751,10 +7751,10 @@
         <v>176</v>
       </c>
       <c r="B181" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="C181" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="D181" t="s">
         <v>509</v>
@@ -7768,7 +7768,7 @@
         <v>177</v>
       </c>
       <c r="C182" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="D182" t="s">
         <v>510</v>
@@ -7779,10 +7779,10 @@
         <v>178</v>
       </c>
       <c r="B183" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C183" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="D183" t="s">
         <v>511</v>
@@ -7796,7 +7796,7 @@
         <v>179</v>
       </c>
       <c r="C184" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="D184" t="s">
         <v>512</v>
@@ -7810,7 +7810,7 @@
         <v>180</v>
       </c>
       <c r="C185" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="D185" t="s">
         <v>513</v>
@@ -7821,10 +7821,10 @@
         <v>181</v>
       </c>
       <c r="B186" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C186" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="D186" t="s">
         <v>514</v>
@@ -7835,10 +7835,10 @@
         <v>182</v>
       </c>
       <c r="B187" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C187" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D187" t="s">
         <v>515</v>
@@ -7849,10 +7849,10 @@
         <v>183</v>
       </c>
       <c r="B188" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C188" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D188" t="s">
         <v>516</v>
@@ -7863,10 +7863,10 @@
         <v>184</v>
       </c>
       <c r="B189" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C189" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="D189" t="s">
         <v>517</v>
@@ -7877,10 +7877,10 @@
         <v>185</v>
       </c>
       <c r="B190" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C190" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="D190" t="s">
         <v>518</v>
@@ -7894,7 +7894,7 @@
         <v>186</v>
       </c>
       <c r="C191" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="D191" t="s">
         <v>519</v>
@@ -7908,7 +7908,7 @@
         <v>187</v>
       </c>
       <c r="C192" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D192" t="s">
         <v>520</v>
@@ -7919,10 +7919,10 @@
         <v>188</v>
       </c>
       <c r="B193" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="C193" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="D193" t="s">
         <v>521</v>
@@ -7936,7 +7936,7 @@
         <v>189</v>
       </c>
       <c r="C194" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="D194" t="s">
         <v>522</v>
@@ -7947,10 +7947,10 @@
         <v>190</v>
       </c>
       <c r="B195" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="C195" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D195" t="s">
         <v>523</v>
@@ -7964,7 +7964,7 @@
         <v>191</v>
       </c>
       <c r="C196" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D196" t="s">
         <v>524</v>
@@ -7975,10 +7975,10 @@
         <v>192</v>
       </c>
       <c r="B197" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="C197" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="D197" t="s">
         <v>525</v>
@@ -7992,7 +7992,7 @@
         <v>193</v>
       </c>
       <c r="C198" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="D198" t="s">
         <v>526</v>
@@ -8006,10 +8006,10 @@
         <v>194</v>
       </c>
       <c r="C199" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="D199" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -8017,10 +8017,10 @@
         <v>195</v>
       </c>
       <c r="B200" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="C200" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D200" t="s">
         <v>527</v>
@@ -8045,10 +8045,10 @@
         <v>197</v>
       </c>
       <c r="B202" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="C202" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="D202" t="s">
         <v>529</v>
@@ -8059,10 +8059,10 @@
         <v>198</v>
       </c>
       <c r="B203" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="C203" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="D203" t="s">
         <v>530</v>
@@ -8073,10 +8073,10 @@
         <v>199</v>
       </c>
       <c r="B204" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="C204" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="D204" t="s">
         <v>531</v>
@@ -8087,10 +8087,10 @@
         <v>200</v>
       </c>
       <c r="B205" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C205" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D205" t="s">
         <v>532</v>
@@ -8101,10 +8101,10 @@
         <v>201</v>
       </c>
       <c r="B206" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="C206" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D206" t="s">
         <v>533</v>
@@ -8115,10 +8115,10 @@
         <v>202</v>
       </c>
       <c r="B207" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="C207" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D207" t="s">
         <v>534</v>
@@ -8132,7 +8132,7 @@
         <v>203</v>
       </c>
       <c r="C208" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D208" t="s">
         <v>535</v>
@@ -8143,10 +8143,10 @@
         <v>204</v>
       </c>
       <c r="B209" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="C209" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D209" t="s">
         <v>536</v>
@@ -8157,10 +8157,10 @@
         <v>205</v>
       </c>
       <c r="B210" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="C210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D210" t="s">
         <v>537</v>
@@ -8174,7 +8174,7 @@
         <v>206</v>
       </c>
       <c r="C211" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="D211" t="s">
         <v>538</v>
@@ -8185,10 +8185,10 @@
         <v>207</v>
       </c>
       <c r="B212" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="C212" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D212" t="s">
         <v>539</v>
@@ -8199,10 +8199,10 @@
         <v>208</v>
       </c>
       <c r="B213" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="C213" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="D213" t="s">
         <v>540</v>
@@ -8213,10 +8213,10 @@
         <v>209</v>
       </c>
       <c r="B214" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="C214" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="D214" t="s">
         <v>541</v>
@@ -8227,10 +8227,10 @@
         <v>210</v>
       </c>
       <c r="B215" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C215" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D215" t="s">
         <v>542</v>
@@ -8241,10 +8241,10 @@
         <v>211</v>
       </c>
       <c r="B216" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="C216" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D216" t="s">
         <v>543</v>
@@ -8255,10 +8255,10 @@
         <v>212</v>
       </c>
       <c r="B217" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C217" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D217" t="s">
         <v>544</v>
@@ -8272,7 +8272,7 @@
         <v>213</v>
       </c>
       <c r="C218" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D218" t="s">
         <v>545</v>
@@ -8283,10 +8283,10 @@
         <v>214</v>
       </c>
       <c r="B219" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="C219" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="D219" t="s">
         <v>546</v>
@@ -8300,7 +8300,7 @@
         <v>215</v>
       </c>
       <c r="C220" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D220" t="s">
         <v>547</v>
@@ -8314,7 +8314,7 @@
         <v>216</v>
       </c>
       <c r="C221" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="D221" t="s">
         <v>548</v>
@@ -8328,7 +8328,7 @@
         <v>217</v>
       </c>
       <c r="C222" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D222" t="s">
         <v>549</v>
@@ -8339,10 +8339,10 @@
         <v>218</v>
       </c>
       <c r="B223" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="C223" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D223" t="s">
         <v>550</v>
@@ -8356,7 +8356,7 @@
         <v>219</v>
       </c>
       <c r="C224" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D224" t="s">
         <v>551</v>
@@ -8367,10 +8367,10 @@
         <v>220</v>
       </c>
       <c r="B225" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="C225" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D225" t="s">
         <v>552</v>
@@ -8384,7 +8384,7 @@
         <v>221</v>
       </c>
       <c r="C226" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D226" t="s">
         <v>553</v>
@@ -8398,7 +8398,7 @@
         <v>222</v>
       </c>
       <c r="C227" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D227" t="s">
         <v>554</v>
@@ -8412,7 +8412,7 @@
         <v>223</v>
       </c>
       <c r="C228" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D228" t="s">
         <v>555</v>
@@ -8423,10 +8423,10 @@
         <v>224</v>
       </c>
       <c r="B229" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="C229" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D229" t="s">
         <v>556</v>
@@ -8440,7 +8440,7 @@
         <v>225</v>
       </c>
       <c r="C230" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D230" t="s">
         <v>557</v>
@@ -8451,10 +8451,10 @@
         <v>226</v>
       </c>
       <c r="B231" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C231" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="D231" t="s">
         <v>558</v>
@@ -8462,16 +8462,16 @@
     </row>
     <row r="232" spans="1:4">
       <c r="A232" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B232" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="C232" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D232" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -8482,7 +8482,7 @@
         <v>227</v>
       </c>
       <c r="C233" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="D233" t="s">
         <v>559</v>
@@ -8496,7 +8496,7 @@
         <v>228</v>
       </c>
       <c r="C234" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="D234" t="s">
         <v>560</v>
@@ -8510,7 +8510,7 @@
         <v>229</v>
       </c>
       <c r="C235" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="D235" t="s">
         <v>561</v>
@@ -8521,10 +8521,10 @@
         <v>230</v>
       </c>
       <c r="B236" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C236" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="D236" t="s">
         <v>562</v>
@@ -8535,10 +8535,10 @@
         <v>231</v>
       </c>
       <c r="B237" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="C237" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="D237" t="s">
         <v>563</v>
@@ -8552,7 +8552,7 @@
         <v>232</v>
       </c>
       <c r="C238" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="D238" t="s">
         <v>564</v>
@@ -8560,16 +8560,16 @@
     </row>
     <row r="239" spans="1:4">
       <c r="A239" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="B239" t="s">
+        <v>939</v>
+      </c>
+      <c r="C239" t="s">
+        <v>941</v>
+      </c>
+      <c r="D239" t="s">
         <v>940</v>
-      </c>
-      <c r="B239" t="s">
-        <v>940</v>
-      </c>
-      <c r="C239" t="s">
-        <v>942</v>
-      </c>
-      <c r="D239" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -8580,10 +8580,10 @@
         <v>233</v>
       </c>
       <c r="C240" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="D240" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -8594,7 +8594,7 @@
         <v>234</v>
       </c>
       <c r="C241" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="D241" t="s">
         <v>565</v>
@@ -8608,7 +8608,7 @@
         <v>235</v>
       </c>
       <c r="C242" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D242" t="s">
         <v>566</v>
@@ -8622,7 +8622,7 @@
         <v>236</v>
       </c>
       <c r="C243" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D243" t="s">
         <v>567</v>
@@ -8636,7 +8636,7 @@
         <v>237</v>
       </c>
       <c r="C244" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="D244" t="s">
         <v>568</v>
@@ -8650,7 +8650,7 @@
         <v>238</v>
       </c>
       <c r="C245" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="D245" t="s">
         <v>569</v>
@@ -8664,7 +8664,7 @@
         <v>239</v>
       </c>
       <c r="C246" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D246" t="s">
         <v>570</v>
@@ -8678,7 +8678,7 @@
         <v>240</v>
       </c>
       <c r="C247" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D247" t="s">
         <v>571</v>
@@ -8689,10 +8689,10 @@
         <v>241</v>
       </c>
       <c r="B248" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="D248" t="s">
         <v>572</v>
@@ -8706,7 +8706,7 @@
         <v>242</v>
       </c>
       <c r="C249" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D249" t="s">
         <v>573</v>
@@ -8717,10 +8717,10 @@
         <v>243</v>
       </c>
       <c r="B250" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C250" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="D250" t="s">
         <v>574</v>
@@ -8731,10 +8731,10 @@
         <v>244</v>
       </c>
       <c r="B251" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="C251" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D251" t="s">
         <v>575</v>
@@ -8745,10 +8745,10 @@
         <v>245</v>
       </c>
       <c r="B252" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C252" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="D252" t="s">
         <v>576</v>
@@ -8762,7 +8762,7 @@
         <v>246</v>
       </c>
       <c r="C253" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="D253" t="s">
         <v>577</v>
@@ -8773,10 +8773,10 @@
         <v>247</v>
       </c>
       <c r="B254" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="C254" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D254" t="s">
         <v>578</v>
@@ -8787,10 +8787,10 @@
         <v>248</v>
       </c>
       <c r="B255" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="C255" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="D255" t="s">
         <v>579</v>
@@ -8801,10 +8801,10 @@
         <v>249</v>
       </c>
       <c r="B256" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="C256" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="D256" t="s">
         <v>580</v>
@@ -8818,7 +8818,7 @@
         <v>250</v>
       </c>
       <c r="C257" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="D257" t="s">
         <v>581</v>
@@ -8832,7 +8832,7 @@
         <v>251</v>
       </c>
       <c r="C258" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="D258" t="s">
         <v>582</v>
@@ -8843,10 +8843,10 @@
         <v>252</v>
       </c>
       <c r="B259" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="C259" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="D259" t="s">
         <v>583</v>
@@ -8857,10 +8857,10 @@
         <v>253</v>
       </c>
       <c r="B260" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="C260" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="D260" t="s">
         <v>584</v>
@@ -8871,10 +8871,10 @@
         <v>254</v>
       </c>
       <c r="B261" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="C261" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="D261" t="s">
         <v>585</v>
@@ -8888,7 +8888,7 @@
         <v>255</v>
       </c>
       <c r="C262" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="D262" t="s">
         <v>586</v>
@@ -8902,7 +8902,7 @@
         <v>256</v>
       </c>
       <c r="C263" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="D263" t="s">
         <v>587</v>
@@ -8916,7 +8916,7 @@
         <v>257</v>
       </c>
       <c r="C264" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="D264" t="s">
         <v>588</v>
@@ -8930,7 +8930,7 @@
         <v>258</v>
       </c>
       <c r="C265" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="D265" t="s">
         <v>589</v>
@@ -8941,10 +8941,10 @@
         <v>259</v>
       </c>
       <c r="B266" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="C266" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="D266" t="s">
         <v>590</v>
@@ -8955,7 +8955,7 @@
         <v>260</v>
       </c>
       <c r="B267" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="C267" t="s">
         <v>260</v>
@@ -8969,10 +8969,10 @@
         <v>261</v>
       </c>
       <c r="B268" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="C268" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="D268" t="s">
         <v>592</v>
@@ -8983,10 +8983,10 @@
         <v>262</v>
       </c>
       <c r="B269" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C269" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="D269" t="s">
         <v>593</v>
@@ -8997,10 +8997,10 @@
         <v>263</v>
       </c>
       <c r="B270" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="C270" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="D270" t="s">
         <v>594</v>
@@ -9014,7 +9014,7 @@
         <v>264</v>
       </c>
       <c r="C271" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="D271" t="s">
         <v>595</v>
@@ -9025,10 +9025,10 @@
         <v>265</v>
       </c>
       <c r="B272" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C272" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="D272" t="s">
         <v>596</v>
@@ -9039,10 +9039,10 @@
         <v>266</v>
       </c>
       <c r="B273" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="C273" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="D273" t="s">
         <v>597</v>
@@ -9053,10 +9053,10 @@
         <v>267</v>
       </c>
       <c r="B274" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C274" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="D274" t="s">
         <v>598</v>
@@ -9067,10 +9067,10 @@
         <v>268</v>
       </c>
       <c r="B275" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C275" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="D275" t="s">
         <v>599</v>
@@ -9084,7 +9084,7 @@
         <v>269</v>
       </c>
       <c r="C276" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="D276" t="s">
         <v>600</v>
@@ -9095,10 +9095,10 @@
         <v>270</v>
       </c>
       <c r="B277" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C277" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="D277" t="s">
         <v>601</v>
@@ -9109,10 +9109,10 @@
         <v>271</v>
       </c>
       <c r="B278" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C278" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="D278" t="s">
         <v>602</v>
@@ -9123,10 +9123,10 @@
         <v>272</v>
       </c>
       <c r="B279" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="C279" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="D279" t="s">
         <v>603</v>
@@ -9137,10 +9137,10 @@
         <v>273</v>
       </c>
       <c r="B280" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="C280" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="D280" t="s">
         <v>604</v>
@@ -9151,10 +9151,10 @@
         <v>274</v>
       </c>
       <c r="B281" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="C281" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="D281" t="s">
         <v>605</v>
@@ -9165,10 +9165,10 @@
         <v>275</v>
       </c>
       <c r="B282" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="C282" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D282" t="s">
         <v>606</v>
@@ -9179,10 +9179,10 @@
         <v>276</v>
       </c>
       <c r="B283" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="C283" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="D283" t="s">
         <v>607</v>
@@ -9196,7 +9196,7 @@
         <v>277</v>
       </c>
       <c r="C284" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="D284" t="s">
         <v>608</v>
@@ -9207,10 +9207,10 @@
         <v>278</v>
       </c>
       <c r="B285" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="C285" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="D285" t="s">
         <v>609</v>
@@ -9224,7 +9224,7 @@
         <v>279</v>
       </c>
       <c r="C286" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="D286" t="s">
         <v>610</v>
@@ -9238,7 +9238,7 @@
         <v>280</v>
       </c>
       <c r="C287" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="D287" t="s">
         <v>611</v>
@@ -9252,7 +9252,7 @@
         <v>281</v>
       </c>
       <c r="C288" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="D288" t="s">
         <v>612</v>
@@ -9263,10 +9263,10 @@
         <v>282</v>
       </c>
       <c r="B289" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="C289" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="D289" t="s">
         <v>613</v>
@@ -9277,7 +9277,7 @@
         <v>283</v>
       </c>
       <c r="B290" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="C290" t="s">
         <v>283</v>
@@ -9294,7 +9294,7 @@
         <v>284</v>
       </c>
       <c r="C291" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="D291" t="s">
         <v>615</v>
@@ -9308,7 +9308,7 @@
         <v>285</v>
       </c>
       <c r="C292" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="D292" t="s">
         <v>616</v>
@@ -9319,10 +9319,10 @@
         <v>286</v>
       </c>
       <c r="B293" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="C293" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D293" t="s">
         <v>617</v>
@@ -9333,10 +9333,10 @@
         <v>287</v>
       </c>
       <c r="B294" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="C294" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="D294" t="s">
         <v>618</v>
@@ -9347,10 +9347,10 @@
         <v>288</v>
       </c>
       <c r="B295" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="C295" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="D295" t="s">
         <v>619</v>
@@ -9364,7 +9364,7 @@
         <v>289</v>
       </c>
       <c r="C296" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="D296" t="s">
         <v>620</v>
@@ -9378,7 +9378,7 @@
         <v>290</v>
       </c>
       <c r="C297" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="D297" t="s">
         <v>621</v>
@@ -9389,10 +9389,10 @@
         <v>291</v>
       </c>
       <c r="B298" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="C298" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="D298" t="s">
         <v>622</v>
@@ -9403,10 +9403,10 @@
         <v>292</v>
       </c>
       <c r="B299" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="C299" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="D299" t="s">
         <v>623</v>
@@ -9417,10 +9417,10 @@
         <v>293</v>
       </c>
       <c r="B300" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="C300" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="D300" t="s">
         <v>624</v>
@@ -9434,7 +9434,7 @@
         <v>294</v>
       </c>
       <c r="C301" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D301" t="s">
         <v>625</v>
@@ -9445,10 +9445,10 @@
         <v>295</v>
       </c>
       <c r="B302" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C302" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D302" t="s">
         <v>626</v>
@@ -9462,7 +9462,7 @@
         <v>296</v>
       </c>
       <c r="C303" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D303" t="s">
         <v>627</v>
@@ -9476,7 +9476,7 @@
         <v>297</v>
       </c>
       <c r="C304" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D304" t="s">
         <v>629</v>
@@ -9490,7 +9490,7 @@
         <v>298</v>
       </c>
       <c r="C305" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="D305" t="s">
         <v>628</v>
@@ -9504,7 +9504,7 @@
         <v>299</v>
       </c>
       <c r="C306" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="D306" t="s">
         <v>630</v>
@@ -9518,7 +9518,7 @@
         <v>300</v>
       </c>
       <c r="C307" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="D307" t="s">
         <v>631</v>
@@ -9546,7 +9546,7 @@
         <v>302</v>
       </c>
       <c r="C309" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="D309" t="s">
         <v>633</v>
@@ -9560,7 +9560,7 @@
         <v>303</v>
       </c>
       <c r="C310" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="D310" t="s">
         <v>634</v>
@@ -9574,7 +9574,7 @@
         <v>304</v>
       </c>
       <c r="C311" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="D311" t="s">
         <v>635</v>
@@ -9588,7 +9588,7 @@
         <v>305</v>
       </c>
       <c r="C312" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="D312" t="s">
         <v>636</v>
@@ -9599,10 +9599,10 @@
         <v>306</v>
       </c>
       <c r="B313" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C313" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="D313" t="s">
         <v>637</v>
@@ -9613,7 +9613,7 @@
         <v>307</v>
       </c>
       <c r="B314" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="C314" t="s">
         <v>307</v>
@@ -9641,10 +9641,10 @@
         <v>309</v>
       </c>
       <c r="B316" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="D316" t="s">
         <v>640</v>
@@ -9655,7 +9655,7 @@
         <v>310</v>
       </c>
       <c r="B317" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="C317" t="s">
         <v>310</v>
@@ -9683,10 +9683,10 @@
         <v>312</v>
       </c>
       <c r="B319" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="C319" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D319" t="s">
         <v>643</v>
@@ -9697,10 +9697,10 @@
         <v>313</v>
       </c>
       <c r="B320" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="C320" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D320" t="s">
         <v>644</v>
@@ -9711,10 +9711,10 @@
         <v>314</v>
       </c>
       <c r="B321" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="C321" s="2" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D321" t="s">
         <v>645</v>
@@ -9753,10 +9753,10 @@
         <v>317</v>
       </c>
       <c r="B324" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="C324" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="D324" t="s">
         <v>648</v>
@@ -9767,10 +9767,10 @@
         <v>318</v>
       </c>
       <c r="B325" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="C325" s="2" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="D325" t="s">
         <v>649</v>
@@ -9781,10 +9781,10 @@
         <v>319</v>
       </c>
       <c r="B326" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="C326" s="2" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="D326" t="s">
         <v>650</v>
@@ -9798,7 +9798,7 @@
         <v>320</v>
       </c>
       <c r="C327" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D327" t="s">
         <v>651</v>
@@ -9809,10 +9809,10 @@
         <v>321</v>
       </c>
       <c r="B328" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="C328" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="D328" t="s">
         <v>652</v>
@@ -9823,10 +9823,10 @@
         <v>322</v>
       </c>
       <c r="B329" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="C329" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="D329" t="s">
         <v>653</v>
@@ -9837,7 +9837,7 @@
         <v>323</v>
       </c>
       <c r="B330" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="C330" t="s">
         <v>323</v>
@@ -9851,7 +9851,7 @@
         <v>324</v>
       </c>
       <c r="B331" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="C331" t="s">
         <v>324</v>
@@ -9868,7 +9868,7 @@
         <v>325</v>
       </c>
       <c r="C332" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="D332" t="s">
         <v>656</v>
@@ -9882,7 +9882,7 @@
         <v>326</v>
       </c>
       <c r="C333" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="D333" t="s">
         <v>657</v>
@@ -9910,7 +9910,7 @@
         <v>328</v>
       </c>
       <c r="C335" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="D335" t="s">
         <v>659</v>
@@ -9924,7 +9924,7 @@
         <v>329</v>
       </c>
       <c r="C336" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="D336" t="s">
         <v>660</v>
@@ -9938,7 +9938,7 @@
         <v>330</v>
       </c>
       <c r="C337" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D337" t="s">
         <v>661</v>
@@ -9949,10 +9949,10 @@
         <v>331</v>
       </c>
       <c r="B338" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="C338" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D338" t="s">
         <v>662</v>
@@ -9963,7 +9963,7 @@
         <v>332</v>
       </c>
       <c r="B339" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="C339" t="s">
         <v>332</v>
@@ -9980,7 +9980,7 @@
         <v>333</v>
       </c>
       <c r="C340" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="D340" t="s">
         <v>664</v>
@@ -9994,7 +9994,7 @@
         <v>334</v>
       </c>
       <c r="C341" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D341" t="s">
         <v>665</v>
@@ -10008,7 +10008,7 @@
         <v>335</v>
       </c>
       <c r="C342" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="D342" t="s">
         <v>666</v>
@@ -10019,10 +10019,10 @@
         <v>336</v>
       </c>
       <c r="B343" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="C343" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="D343" t="s">
         <v>667</v>
@@ -10033,10 +10033,10 @@
         <v>337</v>
       </c>
       <c r="B344" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="C344" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D344" t="s">
         <v>668</v>
@@ -10047,10 +10047,10 @@
         <v>338</v>
       </c>
       <c r="B345" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="C345" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="D345" t="s">
         <v>669</v>
@@ -10061,10 +10061,10 @@
         <v>339</v>
       </c>
       <c r="B346" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="C346" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="D346" t="s">
         <v>670</v>
@@ -10075,10 +10075,10 @@
         <v>340</v>
       </c>
       <c r="B347" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="C347" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D347" t="s">
         <v>671</v>
@@ -10089,10 +10089,10 @@
         <v>341</v>
       </c>
       <c r="B348" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="C348" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D348" t="s">
         <v>672</v>
@@ -10103,10 +10103,10 @@
         <v>342</v>
       </c>
       <c r="B349" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="C349" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D349" t="s">
         <v>673</v>
@@ -10117,10 +10117,10 @@
         <v>343</v>
       </c>
       <c r="B350" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="C350" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="D350" t="s">
         <v>674</v>
@@ -10131,10 +10131,10 @@
         <v>344</v>
       </c>
       <c r="B351" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="C351" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D351" t="s">
         <v>675</v>
@@ -10148,7 +10148,7 @@
         <v>345</v>
       </c>
       <c r="C352" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="D352" t="s">
         <v>676</v>
@@ -10162,7 +10162,7 @@
         <v>346</v>
       </c>
       <c r="C353" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D353" t="s">
         <v>677</v>
@@ -10176,10 +10176,10 @@
         <v>347</v>
       </c>
       <c r="C354" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D354" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="355" spans="1:4">
@@ -10187,10 +10187,10 @@
         <v>348</v>
       </c>
       <c r="B355" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="C355" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D355" t="s">
         <v>678</v>
@@ -10204,7 +10204,7 @@
         <v>349</v>
       </c>
       <c r="C356" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="D356" t="s">
         <v>679</v>
@@ -10218,7 +10218,7 @@
         <v>350</v>
       </c>
       <c r="C357" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="D357" t="s">
         <v>680</v>
@@ -10226,16 +10226,16 @@
     </row>
     <row r="358" spans="1:4">
       <c r="A358" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B358" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C358" t="s">
         <v>1045</v>
       </c>
-      <c r="B358" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C358" t="s">
+      <c r="D358" t="s">
         <v>1046</v>
-      </c>
-      <c r="D358" t="s">
-        <v>1047</v>
       </c>
     </row>
     <row r="359" spans="1:4">
@@ -10243,10 +10243,10 @@
         <v>351</v>
       </c>
       <c r="B359" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C359" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D359" t="s">
         <v>681</v>

</xml_diff>